<commit_message>
Corrected Matrices dimension | Corrected XLS for testing
</commit_message>
<xml_diff>
--- a/xls/time_results.xlsx
+++ b/xls/time_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="27940" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="27880" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tempos" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
   <si>
     <t>BLAS2LU.m</t>
   </si>
@@ -32,24 +32,6 @@
     <t>BLAS3LU.m</t>
   </si>
   <si>
-    <t>4.4142</t>
-  </si>
-  <si>
-    <t>37.7041</t>
-  </si>
-  <si>
-    <t>305.3466</t>
-  </si>
-  <si>
-    <t>0.2961</t>
-  </si>
-  <si>
-    <t>1.5952</t>
-  </si>
-  <si>
-    <t>8.7272</t>
-  </si>
-  <si>
     <t>Time(sec)</t>
   </si>
   <si>
@@ -65,7 +47,31 @@
     <t>with PP</t>
   </si>
   <si>
-    <t>SpeedUp (without_PP/with_PP)</t>
+    <t>1024x1024</t>
+  </si>
+  <si>
+    <t>512x512</t>
+  </si>
+  <si>
+    <t>2048x2048</t>
+  </si>
+  <si>
+    <t>BLAS2LUPP.m</t>
+  </si>
+  <si>
+    <t>Block Size</t>
+  </si>
+  <si>
+    <t>BLAS3LUPP.m</t>
+  </si>
+  <si>
+    <t>Cabe em cache (2MB)</t>
+  </si>
+  <si>
+    <t>SpeedUp (Texe_without_PP/Texec_with_PP)</t>
+  </si>
+  <si>
+    <t>Relative_Error</t>
   </si>
 </sst>
 </file>
@@ -97,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -159,11 +165,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,9 +271,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -194,19 +283,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -486,177 +629,346 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E6:K21"/>
+  <dimension ref="B2:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="6" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E7" s="8" t="s">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="K3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B4" s="13"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="K4" s="13"/>
+      <c r="L4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B5" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="2"/>
+      <c r="K5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="4" t="s">
+      <c r="C6" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="K6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="13"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="1">
-        <v>1024</v>
-      </c>
-      <c r="J8" s="1">
-        <v>2048</v>
-      </c>
-      <c r="K8" s="1">
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E9" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7" t="s">
+      <c r="H11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="8">
+        <v>32</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="R12" s="33"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="8">
+        <v>64</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="R13" s="33"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="8">
+        <v>32</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="R14" s="33"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="8">
+        <v>64</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="R15" s="33"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R16" s="5"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E10" s="9"/>
-      <c r="F10" s="7" t="s">
+      <c r="G18" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B19" s="13"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B20" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="8">
+        <v>32</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="8">
+        <v>64</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B22" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E12" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" s="2" t="s">
+      <c r="C22" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E13" s="9"/>
-      <c r="F13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E17" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E18" s="16"/>
-      <c r="F18" s="13">
-        <v>1024</v>
-      </c>
-      <c r="G18" s="1">
-        <v>2048</v>
-      </c>
-      <c r="H18" s="1">
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E19" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E20" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="8">
+        <v>32</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="8">
+        <v>64</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F7:H8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E11:K11"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="I7:K7"/>
+  <mergeCells count="23">
+    <mergeCell ref="C20:E21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:E23"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:E11"/>
+    <mergeCell ref="C12:E13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:E15"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:E19"/>
+    <mergeCell ref="C3:E4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
BLAS2 and BLAS3 added with pivoting - Maybe final Release
</commit_message>
<xml_diff>
--- a/xls/time_results.xlsx
+++ b/xls/time_results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
   <si>
     <t>BLAS2LU.m</t>
   </si>
@@ -101,19 +101,73 @@
     <t>NÃO CABEM NA CACHE</t>
   </si>
   <si>
-    <t>BLAS2</t>
-  </si>
-  <si>
     <t>Matrix</t>
   </si>
   <si>
-    <t>SpeedUp  Without Using Pivoting</t>
-  </si>
-  <si>
-    <t>BLAS3 (Block Size = 32)</t>
-  </si>
-  <si>
-    <t>BLAS3 (Block Size = 64)</t>
+    <t>5.5652e-14</t>
+  </si>
+  <si>
+    <t>4.0152e-14</t>
+  </si>
+  <si>
+    <t>4.6326e-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.2063e-14</t>
+  </si>
+  <si>
+    <t>3.6586e-13</t>
+  </si>
+  <si>
+    <t>5.1319e-13</t>
+  </si>
+  <si>
+    <t>1.8056e-13</t>
+  </si>
+  <si>
+    <t>5.4729e-13</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>SpeedUp  Analysis: Without PP VS With PP</t>
+  </si>
+  <si>
+    <t>BLAS2LUPP</t>
+  </si>
+  <si>
+    <t>BLAS3LUPP (b = 32)</t>
+  </si>
+  <si>
+    <t>BLAS3LUPP (b = 64)</t>
+  </si>
+  <si>
+    <t>1.7302e-15</t>
+  </si>
+  <si>
+    <t>1.0989e-15</t>
+  </si>
+  <si>
+    <t>1.4381e-15</t>
+  </si>
+  <si>
+    <t>1.8987e-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.6600e-15</t>
+  </si>
+  <si>
+    <t>5.0550e-15</t>
+  </si>
+  <si>
+    <t>3.4517e-15</t>
+  </si>
+  <si>
+    <t>2.2303e-15</t>
+  </si>
+  <si>
+    <t>SpeedUp  Analysis: BLAS2LU/BLAS3LU</t>
   </si>
 </sst>
 </file>
@@ -159,7 +213,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -285,15 +339,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -301,14 +374,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,28 +383,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -359,14 +408,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,6 +453,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -385,15 +465,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -410,21 +481,60 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -466,7 +576,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2000" baseline="0"/>
-              <a:t>Performance SpeedUp Without Using Pivoting - BLAS2 VS BLAS3</a:t>
+              <a:t>Performance SpeedUp Analysis (Without PP VS With PP)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -475,8 +585,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.221058128833922"/>
-          <c:y val="0.0324288076707175"/>
+          <c:x val="0.221058086255696"/>
+          <c:y val="0.0498154397790327"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -503,11 +613,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tempos!$M$35</c:f>
+              <c:f>Tempos!$J$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BLAS2</c:v>
+                  <c:v>BLAS2LUPP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -520,9 +630,31 @@
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tempos!$L$36:$L$39</c:f>
+              <c:f>Tempos!$I$25:$I$28</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -542,7 +674,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tempos!$M$36:$M$39</c:f>
+              <c:f>Tempos!$J$25:$J$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -567,19 +699,41 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tempos!$N$35</c:f>
+              <c:f>Tempos!$K$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BLAS3 (Block Size = 32)</c:v>
+                  <c:v>BLAS3LUPP (b = 32)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tempos!$L$36:$L$39</c:f>
+              <c:f>Tempos!$I$25:$I$28</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -599,10 +753,22 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tempos!$N$36:$N$39</c:f>
+              <c:f>Tempos!$K$25:$K$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.597864768683274</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.381555153707052</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.11695906432749</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.84828973843058</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -612,19 +778,41 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tempos!$O$35</c:f>
+              <c:f>Tempos!$L$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BLAS3 (Block Size = 64)</c:v>
+                  <c:v>BLAS3LUPP (b = 64)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tempos!$L$36:$L$39</c:f>
+              <c:f>Tempos!$I$25:$I$28</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -644,10 +832,22 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tempos!$O$36:$O$39</c:f>
+              <c:f>Tempos!$L$25:$L$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.794871794871795</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.156040268456376</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.693027210884353</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.45640219952867</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -661,11 +861,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2046309248"/>
-        <c:axId val="-2045189968"/>
+        <c:axId val="2100624288"/>
+        <c:axId val="2127042928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2046309248"/>
+        <c:axId val="2100624288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,7 +885,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2045189968"/>
+        <c:crossAx val="2127042928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -693,10 +893,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2045189968"/>
+        <c:axId val="2127042928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.25"/>
+          <c:max val="13.0"/>
           <c:min val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -727,8 +927,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0200186614173228"/>
-              <c:y val="0.349685949660917"/>
+              <c:x val="0.0152842671339787"/>
+              <c:y val="0.336163064043446"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -747,10 +947,10 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2046309248"/>
+        <c:crossAx val="2100624288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.02"/>
+        <c:majorUnit val="1.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -793,20 +993,455 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+              <a:t>SpeedUp Comparision Levels:  BLAS2LUPP VS BLAS3LUPP </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.231762165996863"/>
+          <c:y val="0.0498154397790327"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.113360866141732"/>
+          <c:y val="0.156806244595148"/>
+          <c:w val="0.694874094488189"/>
+          <c:h val="0.774285194119521"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tempos!$AC$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BLAS2LUPP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tempos!$AB$18:$AB$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256x256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512x512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024x1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048x2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tempos!$AC$18:$AC$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tempos!$AD$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BLAS3LUPP (b = 32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tempos!$AB$18:$AB$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256x256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512x512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024x1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048x2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tempos!$AD$18:$AD$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.476614699331848</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.003714403631861</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.826094137076796</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.832331078259417</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tempos!$AE$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BLAS3LUPP (b = 64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tempos!$AB$18:$AB$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>256x256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512x512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024x1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048x2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tempos!$AE$18:$AE$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.578571428571429</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.581073896863371</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.303061986557132</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.239888501227594</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2123599776"/>
+        <c:axId val="2123602624"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2123599776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2123602624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2123602624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3.5"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1600"/>
+                  <a:t>SpeedUp</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1600" baseline="0"/>
+                  <a:t> (BLAS2LUPP/BLAS3LUPP)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0176594975735563"/>
+              <c:y val="0.32843566008306"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2123599776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.5"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.825980395161124"/>
+          <c:y val="0.455869526130642"/>
+          <c:w val="0.158898517431557"/>
+          <c:h val="0.160637507016825"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup paperSize="9" orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>61610</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>107275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>1134534</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>810639</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>196175</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -822,6 +1457,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>459360</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>27020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>445849</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>115920</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1093,558 +1760,771 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:S39"/>
+  <dimension ref="B3:AF39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="O24" zoomScale="108" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B3" s="40" t="s">
+    <row r="3" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="34" t="s">
+      <c r="D3" s="40"/>
+      <c r="E3" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="35"/>
       <c r="G3" s="35"/>
-      <c r="H3" s="36"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B4" s="41"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="11" t="s">
+      <c r="H3" s="35"/>
+      <c r="I3" s="36"/>
+      <c r="L3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="M3" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B4" s="38"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="12" t="s">
+      <c r="L4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="29"/>
+    </row>
+    <row r="5" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B5" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="9">
+      <c r="D5" s="44"/>
+      <c r="E5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="21">
         <v>5.4699999999999999E-2</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="1">
         <v>0.40539999999999998</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="1">
         <v>4.1318000000000001</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="1">
         <v>33.654200000000003</v>
       </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+      <c r="L5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="2">
+      <c r="D6" s="43"/>
+      <c r="E6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="1">
         <v>6.6299999999999998E-2</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="1">
         <v>0.48549999999999999</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="1">
         <v>4.4227999999999996</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="1">
         <v>35.101599999999998</v>
       </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B7" s="4"/>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B10" s="40" t="s">
+      <c r="L6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="29"/>
+    </row>
+    <row r="7" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B7" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="E7" s="4">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2.81E-2</v>
+      </c>
+      <c r="G7" s="22">
+        <v>5.5300000000000002E-2</v>
+      </c>
+      <c r="H7" s="22">
+        <v>0.2394</v>
+      </c>
+      <c r="I7" s="22">
+        <v>1.4910000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B8" s="45"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="4">
+        <v>64</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.3400000000000001E-2</v>
+      </c>
+      <c r="G8" s="22">
+        <v>5.96E-2</v>
+      </c>
+      <c r="H8" s="22">
+        <v>0.23519999999999999</v>
+      </c>
+      <c r="I8" s="22">
+        <v>1.1456999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B9" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="4">
+        <v>32</v>
+      </c>
+      <c r="F9" s="28">
+        <v>4.4900000000000002E-2</v>
+      </c>
+      <c r="G9" s="23">
+        <v>0.24229999999999999</v>
+      </c>
+      <c r="H9" s="23">
+        <v>2.4220000000000002</v>
+      </c>
+      <c r="I9" s="23">
+        <v>19.1568</v>
+      </c>
+    </row>
+    <row r="10" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B10" s="45"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="4">
+        <v>64</v>
+      </c>
+      <c r="F10" s="28">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0.18809999999999999</v>
+      </c>
+      <c r="H10" s="23">
+        <v>1.339</v>
+      </c>
+      <c r="I10" s="23">
+        <v>10.834199999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B12" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C12" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="30" t="s">
+      <c r="D12" s="40"/>
+      <c r="E12" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B11" s="41"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="11" t="s">
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+    </row>
+    <row r="13" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B13" s="38"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="G13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="H13" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="I13" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="12" t="s">
+    <row r="14" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B14" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C14" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="17" t="s">
+      <c r="D14" s="32"/>
+      <c r="E14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G14" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="I14" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="K12" s="9" t="s">
+    </row>
+    <row r="15" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B15" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B16" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="33"/>
+      <c r="E16" s="4">
+        <v>32</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="R16" s="2"/>
+      <c r="S16" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="T16" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="U16" s="59"/>
+      <c r="V16" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="W16" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="X16" s="35"/>
+      <c r="Y16" s="35"/>
+      <c r="Z16" s="36"/>
+      <c r="AB16" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC16" s="48"/>
+      <c r="AD16" s="48"/>
+      <c r="AE16" s="48"/>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B17" s="46"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="4">
+        <v>64</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="S17" s="38"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="60"/>
+      <c r="V17" s="38"/>
+      <c r="W17" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+      <c r="X17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC17" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF17" s="17"/>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B18" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="33"/>
+      <c r="E18" s="4">
+        <v>32</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="S18" s="47"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="58"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="25"/>
+      <c r="X18" s="28"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="28"/>
+      <c r="AB18" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC18" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="9">
+        <f>W19/W20</f>
+        <v>1.4766146993318485</v>
+      </c>
+      <c r="AE18" s="9">
+        <f>W19/W21</f>
+        <v>1.5785714285714285</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B19" s="46"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="4">
+        <v>64</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="S19" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="T19" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="14"/>
-      <c r="K13" s="13" t="s">
+      <c r="U19" s="56"/>
+      <c r="V19" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="W19" s="28">
+        <v>6.6299999999999998E-2</v>
+      </c>
+      <c r="X19" s="28">
+        <v>0.48549999999999999</v>
+      </c>
+      <c r="Y19" s="28">
+        <v>4.4227999999999996</v>
+      </c>
+      <c r="Z19" s="28">
+        <v>35.101599999999998</v>
+      </c>
+      <c r="AB19" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="30"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="14"/>
-      <c r="K14" s="13" t="s">
+      <c r="AC19" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="9">
+        <f>X19/X20</f>
+        <v>2.0037144036318613</v>
+      </c>
+      <c r="AE19" s="9">
+        <f>X19/X21</f>
+        <v>2.5810738968633706</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="S20" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="T20" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="U20" s="50"/>
+      <c r="V20" s="23">
+        <v>32</v>
+      </c>
+      <c r="W20" s="28">
+        <v>4.4900000000000002E-2</v>
+      </c>
+      <c r="X20" s="23">
+        <v>0.24229999999999999</v>
+      </c>
+      <c r="Y20" s="23">
+        <v>2.4220000000000002</v>
+      </c>
+      <c r="Z20" s="23">
+        <v>19.1568</v>
+      </c>
+      <c r="AB20" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="K15" s="13" t="s">
+      <c r="AC20" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="9">
+        <f>Y19/Y20</f>
+        <v>1.8260941370767958</v>
+      </c>
+      <c r="AE20" s="9">
+        <f>Y19/Y21</f>
+        <v>3.303061986557132</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="S21" s="54"/>
+      <c r="T21" s="51"/>
+      <c r="U21" s="52"/>
+      <c r="V21" s="23">
+        <v>64</v>
+      </c>
+      <c r="W21" s="28">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="X21" s="23">
+        <v>0.18809999999999999</v>
+      </c>
+      <c r="Y21" s="23">
+        <v>1.339</v>
+      </c>
+      <c r="Z21" s="23">
+        <v>10.834199999999999</v>
+      </c>
+      <c r="AB21" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="30"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="R16" s="3"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B18" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B19" s="41"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="8" t="s">
+      <c r="AC21" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="9">
+        <f>Z19/Z20</f>
+        <v>1.8323310782594169</v>
+      </c>
+      <c r="AE21" s="9">
+        <f>Z19/Z21</f>
+        <v>3.2398885012275942</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="I23" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="I24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L24" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="I25" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="J25" s="9">
+        <f>F6/F5</f>
+        <v>1.2120658135283364</v>
+      </c>
+      <c r="K25" s="9">
+        <f>F9/F7</f>
+        <v>1.5978647686832741</v>
+      </c>
+      <c r="L25" s="9">
+        <f>F10/F8</f>
+        <v>1.7948717948717949</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="I26" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="J26" s="9">
+        <f>G6/G5</f>
+        <v>1.1975826344351259</v>
+      </c>
+      <c r="K26" s="9">
+        <f>G9/G7</f>
+        <v>4.3815551537070521</v>
+      </c>
+      <c r="L26" s="9">
+        <f>G10/G8</f>
+        <v>3.1560402684563758</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="I27" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="J27" s="9">
+        <f>H6/H5</f>
+        <v>1.0704293528244346</v>
+      </c>
+      <c r="K27" s="9">
+        <f>H9/H7</f>
+        <v>10.116959064327485</v>
+      </c>
+      <c r="L27" s="9">
+        <f>H10/H8</f>
+        <v>5.6930272108843534</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="I28" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B20" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="6">
-        <v>32</v>
-      </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B21" s="49"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="6">
-        <v>64</v>
-      </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="6">
-        <v>32</v>
-      </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B23" s="49"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="6">
-        <v>64</v>
-      </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B26" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="43"/>
-      <c r="E26" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="39"/>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B27" s="41"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B28" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="50"/>
-      <c r="E28" s="6">
-        <v>32</v>
-      </c>
-      <c r="F28" s="18"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B29" s="49"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="6">
-        <v>64</v>
-      </c>
-      <c r="F29" s="18"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B30" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="50"/>
-      <c r="E30" s="6">
-        <v>32</v>
-      </c>
-      <c r="F30" s="18"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B31" s="49"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="6">
-        <v>64</v>
-      </c>
-      <c r="F31" s="18"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="J28" s="9">
+        <f>I6/I5</f>
+        <v>1.043008004944405</v>
+      </c>
+      <c r="K28" s="9">
+        <f>I9/I7</f>
+        <v>12.848289738430584</v>
+      </c>
+      <c r="L28" s="9">
+        <f>I10/I8</f>
+        <v>9.4564021995286716</v>
+      </c>
+    </row>
+    <row r="32" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="29"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="L34" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="M34" s="31"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="20"/>
-      <c r="S34" s="20"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B35" s="29"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="L35" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M35" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="N35" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O35" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="P35" s="21"/>
-      <c r="Q35" s="21"/>
-      <c r="R35" s="21"/>
-      <c r="S35" s="21"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+      <c r="S35" s="12"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="L36" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="M36" s="18">
-        <f>E6/E5</f>
-        <v>1.2120658135283364</v>
-      </c>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="L37" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="M37" s="18">
-        <f>F6/F5</f>
-        <v>1.1975826344351259</v>
-      </c>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
-      <c r="S37" s="3"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="L38" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="M38" s="18">
-        <f>G6/G5</f>
-        <v>1.0704293528244346</v>
-      </c>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="L39" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="M39" s="18">
-        <f>H6/H5</f>
-        <v>1.043008004944405</v>
-      </c>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="C28:D29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:D27"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:D11"/>
+  <mergeCells count="32">
+    <mergeCell ref="AB16:AE16"/>
+    <mergeCell ref="S16:S17"/>
+    <mergeCell ref="T16:U17"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="W16:Z16"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="S20:S21"/>
+    <mergeCell ref="T20:U21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:D13"/>
     <mergeCell ref="C3:D4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="C16:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>